<commit_message>
Update sheet with index page, update yaml troubleshooter
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjgar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjgar\Documents\RPI\clubs and activities\Metallography\course-intro-ml-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADE9AB6-29C8-4A57-815E-E89D2C9AE7F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424C673B-7A29-4F6B-95B9-D809C2BA2604}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3959" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3976" uniqueCount="758">
   <si>
     <t>MGMT6560-fa19</t>
   </si>
@@ -2311,25 +2311,13 @@
     <t>Landing page description:</t>
   </si>
   <si>
-    <t>divider:</t>
-  </si>
-  <si>
     <t>search:</t>
   </si>
   <si>
-    <t>- title:</t>
-  </si>
-  <si>
     <t>not_numbered:</t>
   </si>
   <si>
-    <t>/index</t>
-  </si>
-  <si>
     <t>url:</t>
-  </si>
-  <si>
-    <t>Home</t>
   </si>
   <si>
     <t>The [Schedule](https://rpi-data.github.io/course-intro-ml-app/schedule.html) for the course.
@@ -2346,6 +2334,30 @@
   </si>
   <si>
     <t>=configuration!B14</t>
+  </si>
+  <si>
+    <t>external:</t>
+  </si>
+  <si>
+    <t>title:</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>baseurl</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
 </sst>
 </file>
@@ -2486,7 +2498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2560,6 +2572,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2567,8 +2582,8 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2889,8 +2904,8 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1484375" defaultRowHeight="15" customHeight="1"/>
@@ -3005,23 +3020,23 @@
       <c r="A14" s="36" t="s">
         <v>722</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="40" t="s">
         <v>724</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
     </row>
     <row r="15" spans="1:5" s="8" customFormat="1" ht="99" customHeight="1">
       <c r="A15" s="36" t="s">
         <v>743</v>
       </c>
-      <c r="B15" s="37" t="s">
-        <v>751</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
+      <c r="B15" s="40" t="s">
+        <v>747</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:5" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="1"/>
@@ -3155,7 +3170,7 @@
       <c r="A32" s="13" t="s">
         <v>698</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="28" t="s">
         <v>678</v>
       </c>
     </row>
@@ -3171,7 +3186,7 @@
       <c r="A34" s="13" t="s">
         <v>698</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="28" t="s">
         <v>679</v>
       </c>
     </row>
@@ -3187,7 +3202,7 @@
       <c r="A36" s="13" t="s">
         <v>698</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="28" t="s">
         <v>680</v>
       </c>
     </row>
@@ -3200,9 +3215,12 @@
     <hyperlink ref="B8" r:id="rId1" xr:uid="{042009D7-9FD9-483E-8B74-03E32AAD5484}"/>
     <hyperlink ref="B27" r:id="rId2" xr:uid="{69EC54D9-7D43-492D-9D92-266E9DF0F5C0}"/>
     <hyperlink ref="B12" r:id="rId3" xr:uid="{CE8243A2-6234-41E5-8DB9-AB660C9B9DAD}"/>
+    <hyperlink ref="B36" r:id="rId4" xr:uid="{51B2D1FD-2C81-4C95-9DFD-0AACC3F1B2EF}"/>
+    <hyperlink ref="B34" r:id="rId5" location="recent=true" xr:uid="{1DF8FC81-1E99-4855-8529-7226CC41AC58}"/>
+    <hyperlink ref="B32" r:id="rId6" xr:uid="{4BB445A6-0E2F-4B11-A87B-D3AD30B9BD77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -38962,15 +38980,71 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65506883-8C0B-4B4B-9CDC-69050B8D6DCA}">
-  <dimension ref="A5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="2" max="2" width="8.796875" style="43"/>
+  </cols>
   <sheetData>
-    <row r="5" s="8" customFormat="1"/>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B1" s="43" t="str">
+        <f>configuration!B2</f>
+        <v>MGMT6560-fa19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>753</v>
+      </c>
+      <c r="B2" s="30" t="str">
+        <f>configuration!B7</f>
+        <v>Jason Kuruzovich</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>754</v>
+      </c>
+      <c r="B3" s="30" t="str">
+        <f>configuration!B8</f>
+        <v>kuruzj@rpi.edu</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>755</v>
+      </c>
+      <c r="B4" s="30" t="str">
+        <f>configuration!B18</f>
+        <v>Welcome to Technology Fundamentals for Business Analytics. We are going to familiarize you with all phases of the data science lifecycle and a wide variety of the technologies used.</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="8" customFormat="1">
+      <c r="A5" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="B5" s="30" t="str">
+        <f>configuration!B19</f>
+        <v xml:space="preserve">/course-intro-ml-app  </v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>757</v>
+      </c>
+      <c r="B6" s="30" t="str">
+        <f>configuration!B20</f>
+        <v xml:space="preserve">https://rpi-data.github.io  </v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38978,61 +39052,128 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D008F881-5C6F-4157-A868-DE4C1A16983B}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="14.44921875" customWidth="1"/>
+    <col min="2" max="2" width="8.796875" style="43"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="37" t="s">
+        <v>744</v>
+      </c>
+      <c r="B1" s="38" t="str">
+        <f>configuration!B23</f>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="39" t="s">
+        <v>751</v>
+      </c>
+      <c r="B2" s="43" t="str">
+        <f>configuration!B31</f>
+        <v>GitHub Repository</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
         <v>746</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B3" s="30" t="str">
+        <f>configuration!B32</f>
+        <v>https://github.com/RPI-DATA/jupyter-book</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="8" customFormat="1">
+      <c r="A4" s="8" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="40" t="s">
-        <v>749</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="40" t="s">
-        <v>747</v>
-      </c>
-      <c r="B3" s="40"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
+      <c r="B4" s="43" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="37" t="s">
+        <v>745</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="39" t="s">
+        <v>751</v>
+      </c>
+      <c r="B6" s="30" t="str">
+        <f>configuration!B33</f>
+        <v>Colab</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8" t="s">
         <v>746</v>
       </c>
-      <c r="B5" s="40"/>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="40" t="s">
+      <c r="B7" s="30" t="str">
+        <f>configuration!B34</f>
+        <v>https://colab.research.google.com/notebooks/welcome.ipynb#recent=true</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8" t="s">
+        <v>750</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="37" t="s">
         <v>745</v>
       </c>
-      <c r="B6" s="40"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="40" t="s">
-        <v>744</v>
-      </c>
-      <c r="B8" s="40"/>
+      <c r="B9" s="44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="39" t="s">
+        <v>751</v>
+      </c>
+      <c r="B10" s="30" t="str">
+        <f>configuration!B35</f>
+        <v>Slack</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="B11" s="30" t="str">
+        <f>configuration!B36</f>
+        <v>https://rpi-data.slack.com/messages</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8" t="s">
+        <v>750</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="37" t="s">
+        <v>745</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39054,7 +39195,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="78">
       <c r="A1" s="34" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -39154,7 +39295,7 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="30" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
     </row>
   </sheetData>
@@ -39528,10 +39669,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A5" s="38">
+      <c r="A5" s="41">
         <v>43709</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="42"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="10">
@@ -39574,10 +39715,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A11" s="38">
+      <c r="A11" s="41">
         <v>43739</v>
       </c>
-      <c r="B11" s="39"/>
+      <c r="B11" s="42"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="10">
@@ -39628,10 +39769,10 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A18" s="38">
+      <c r="A18" s="41">
         <v>43770</v>
       </c>
-      <c r="B18" s="39"/>
+      <c r="B18" s="42"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1">
       <c r="A19" s="12" t="s">
@@ -39698,10 +39839,10 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A27" s="38">
+      <c r="A27" s="41">
         <v>43800</v>
       </c>
-      <c r="B27" s="39"/>
+      <c r="B27" s="42"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1">
       <c r="A28" s="10">
@@ -39784,10 +39925,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A38" s="38">
+      <c r="A38" s="41">
         <v>43831</v>
       </c>
-      <c r="B38" s="39"/>
+      <c r="B38" s="42"/>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1">
       <c r="A39" s="12" t="s">
@@ -39838,10 +39979,10 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A45" s="38">
+      <c r="A45" s="41">
         <v>43862</v>
       </c>
-      <c r="B45" s="39"/>
+      <c r="B45" s="42"/>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1">
       <c r="A46" s="10">
@@ -39868,10 +40009,10 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A49" s="38">
+      <c r="A49" s="41">
         <v>43891</v>
       </c>
-      <c r="B49" s="39"/>
+      <c r="B49" s="42"/>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1">
       <c r="A50" s="10">
@@ -39946,10 +40087,10 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A59" s="38">
+      <c r="A59" s="41">
         <v>43922</v>
       </c>
-      <c r="B59" s="39"/>
+      <c r="B59" s="42"/>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1">
       <c r="A60" s="10">
@@ -39992,10 +40133,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A65" s="38">
+      <c r="A65" s="41">
         <v>43952</v>
       </c>
-      <c r="B65" s="39"/>
+      <c r="B65" s="42"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1">
       <c r="A66" s="12" t="s">

</xml_diff>